<commit_message>
main and new forecast
</commit_message>
<xml_diff>
--- a/Exports/TeamExport_A46051_Alpha_M_Period 1.xlsx
+++ b/Exports/TeamExport_A46051_Alpha_M_Period 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Anno III\UCSD\112\Markstrat\Reports\Exports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Anno III\UCSD\112\Markstrat\Code\Exports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{120714BD-A888-4349-860E-DC7BDA0A841F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19F0F70-9081-43B9-A6FA-352EA3DC0B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Firm" sheetId="1" r:id="rId1"/>
@@ -2496,18 +2496,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -9895,7 +9884,7 @@
       <c r="L152" s="331"/>
       <c r="M152" s="332"/>
     </row>
-    <row r="153" spans="1:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:15" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B153" s="82"/>
       <c r="D153" s="328"/>
       <c r="E153" s="329"/>
@@ -10508,7 +10497,7 @@
       <c r="L187" s="331"/>
       <c r="M187" s="332"/>
     </row>
-    <row r="188" spans="1:13" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:13" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B188" s="82"/>
       <c r="D188" s="328"/>
       <c r="E188" s="329"/>
@@ -14313,7 +14302,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="454" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B454" s="82"/>
       <c r="D454" s="328" t="s">
         <v>54</v>
@@ -14477,7 +14466,7 @@
       <c r="J463" s="4"/>
       <c r="K463" s="3"/>
     </row>
-    <row r="464" spans="1:11" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:11" s="81" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B464" s="82"/>
       <c r="D464" s="328" t="s">
         <v>54</v>
@@ -16674,6 +16663,21 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="D563:E563"/>
+    <mergeCell ref="D507:E507"/>
+    <mergeCell ref="F551:H551"/>
+    <mergeCell ref="I551:K551"/>
+    <mergeCell ref="D552:E552"/>
+    <mergeCell ref="L551:N551"/>
+    <mergeCell ref="D515:E515"/>
+    <mergeCell ref="D525:E525"/>
+    <mergeCell ref="D533:E533"/>
+    <mergeCell ref="D541:E541"/>
+    <mergeCell ref="F187:I187"/>
+    <mergeCell ref="J187:M187"/>
+    <mergeCell ref="D152:E153"/>
+    <mergeCell ref="F152:I152"/>
+    <mergeCell ref="J152:M152"/>
     <mergeCell ref="D383:E383"/>
     <mergeCell ref="D454:E454"/>
     <mergeCell ref="D464:E464"/>
@@ -16688,21 +16692,6 @@
     <mergeCell ref="D372:E372"/>
     <mergeCell ref="D187:E188"/>
     <mergeCell ref="D418:E418"/>
-    <mergeCell ref="F187:I187"/>
-    <mergeCell ref="J187:M187"/>
-    <mergeCell ref="D152:E153"/>
-    <mergeCell ref="F152:I152"/>
-    <mergeCell ref="J152:M152"/>
-    <mergeCell ref="L551:N551"/>
-    <mergeCell ref="D515:E515"/>
-    <mergeCell ref="D525:E525"/>
-    <mergeCell ref="D533:E533"/>
-    <mergeCell ref="D541:E541"/>
-    <mergeCell ref="D563:E563"/>
-    <mergeCell ref="D507:E507"/>
-    <mergeCell ref="F551:H551"/>
-    <mergeCell ref="I551:K551"/>
-    <mergeCell ref="D552:E552"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -16713,8 +16702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE45BB9-6FD3-43D9-B256-CDED79E8D3DD}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="K13" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="H12" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17249,7 +17238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O592"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N427" sqref="N427"/>
     </sheetView>
   </sheetViews>
@@ -24228,6 +24217,33 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="D362:E362"/>
+    <mergeCell ref="D372:E372"/>
+    <mergeCell ref="D187:E188"/>
+    <mergeCell ref="F187:I187"/>
+    <mergeCell ref="J187:M187"/>
+    <mergeCell ref="D223:E223"/>
+    <mergeCell ref="D296:E296"/>
+    <mergeCell ref="D152:E153"/>
+    <mergeCell ref="F152:I152"/>
+    <mergeCell ref="J152:M152"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="D383:E383"/>
+    <mergeCell ref="D454:E454"/>
+    <mergeCell ref="D464:E464"/>
+    <mergeCell ref="D499:E499"/>
+    <mergeCell ref="D507:E507"/>
+    <mergeCell ref="D418:E418"/>
+    <mergeCell ref="D515:E515"/>
+    <mergeCell ref="D525:E525"/>
+    <mergeCell ref="D533:E533"/>
+    <mergeCell ref="F551:H551"/>
+    <mergeCell ref="I551:K551"/>
+    <mergeCell ref="D541:E541"/>
     <mergeCell ref="D572:E572"/>
     <mergeCell ref="L551:N551"/>
     <mergeCell ref="D552:E552"/>
@@ -24236,33 +24252,6 @@
     <mergeCell ref="H571:I571"/>
     <mergeCell ref="J571:K571"/>
     <mergeCell ref="L571:M571"/>
-    <mergeCell ref="D515:E515"/>
-    <mergeCell ref="D525:E525"/>
-    <mergeCell ref="D533:E533"/>
-    <mergeCell ref="F551:H551"/>
-    <mergeCell ref="I551:K551"/>
-    <mergeCell ref="D541:E541"/>
-    <mergeCell ref="D383:E383"/>
-    <mergeCell ref="D454:E454"/>
-    <mergeCell ref="D464:E464"/>
-    <mergeCell ref="D499:E499"/>
-    <mergeCell ref="D507:E507"/>
-    <mergeCell ref="D418:E418"/>
-    <mergeCell ref="D152:E153"/>
-    <mergeCell ref="F152:I152"/>
-    <mergeCell ref="J152:M152"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D116:E116"/>
-    <mergeCell ref="D362:E362"/>
-    <mergeCell ref="D372:E372"/>
-    <mergeCell ref="D187:E188"/>
-    <mergeCell ref="F187:I187"/>
-    <mergeCell ref="J187:M187"/>
-    <mergeCell ref="D223:E223"/>
-    <mergeCell ref="D296:E296"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>